<commit_message>
Consumer Payments TestCases Separated and Added Bulkdata
</commit_message>
<xml_diff>
--- a/Data Files/Certpay/CertpayTestdataN.xlsx
+++ b/Data Files/Certpay/CertpayTestdataN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12575" firstSheet="11" activeTab="15"/>
+    <workbookView windowWidth="23040" windowHeight="9335" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="SingleBureaSingleLineAmx" sheetId="7" r:id="rId1"/>
@@ -745,7 +745,7 @@
     <t>5474397016786986</t>
   </si>
   <si>
-    <t>Master</t>
+    <t>Mastercard</t>
   </si>
   <si>
     <t>5567887196285070</t>
@@ -1393,11 +1393,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1423,21 +1423,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1459,7 +1452,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1489,61 +1497,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1558,8 +1513,46 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1574,7 +1567,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1586,7 +1609,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1598,163 +1747,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1765,15 +1758,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1801,6 +1785,50 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1812,15 +1840,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1839,175 +1858,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2340,13 +2333,14 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="14" max="14" width="17.4259259259259" customWidth="1"/>
+    <col min="16" max="16" width="16.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -7816,7 +7810,7 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7922,7 +7916,7 @@
         <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -7972,7 +7966,7 @@
         <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -8022,7 +8016,7 @@
         <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -8072,7 +8066,7 @@
         <v>25</v>
       </c>
       <c r="P5" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -8122,7 +8116,7 @@
         <v>25</v>
       </c>
       <c r="P6" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -8172,7 +8166,7 @@
         <v>25</v>
       </c>
       <c r="P7" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -8222,7 +8216,7 @@
         <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -8272,7 +8266,7 @@
         <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -8322,7 +8316,7 @@
         <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -8372,7 +8366,7 @@
         <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -8422,7 +8416,7 @@
         <v>25</v>
       </c>
       <c r="P12" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -8472,7 +8466,7 @@
         <v>25</v>
       </c>
       <c r="P13" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -8522,7 +8516,7 @@
         <v>25</v>
       </c>
       <c r="P14" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -8572,7 +8566,7 @@
         <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -8622,7 +8616,7 @@
         <v>25</v>
       </c>
       <c r="P16" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -8672,7 +8666,7 @@
         <v>25</v>
       </c>
       <c r="P17" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -8722,7 +8716,7 @@
         <v>25</v>
       </c>
       <c r="P18" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -8772,7 +8766,7 @@
         <v>25</v>
       </c>
       <c r="P19" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -8822,7 +8816,7 @@
         <v>25</v>
       </c>
       <c r="P20" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -8872,7 +8866,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -8922,7 +8916,7 @@
         <v>25</v>
       </c>
       <c r="P22" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -8972,7 +8966,7 @@
         <v>25</v>
       </c>
       <c r="P23" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -9022,7 +9016,7 @@
         <v>25</v>
       </c>
       <c r="P24" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -9072,7 +9066,7 @@
         <v>25</v>
       </c>
       <c r="P25" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -9122,7 +9116,7 @@
         <v>25</v>
       </c>
       <c r="P26" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -9172,7 +9166,7 @@
         <v>25</v>
       </c>
       <c r="P27" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -9222,7 +9216,7 @@
         <v>25</v>
       </c>
       <c r="P28" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -9272,7 +9266,7 @@
         <v>25</v>
       </c>
       <c r="P29" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -9322,7 +9316,7 @@
         <v>25</v>
       </c>
       <c r="P30" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -9372,7 +9366,7 @@
         <v>25</v>
       </c>
       <c r="P31" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -9422,7 +9416,7 @@
         <v>25</v>
       </c>
       <c r="P32" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -9472,7 +9466,7 @@
         <v>25</v>
       </c>
       <c r="P33" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -9522,7 +9516,7 @@
         <v>25</v>
       </c>
       <c r="P34" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -9572,7 +9566,7 @@
         <v>25</v>
       </c>
       <c r="P35" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -9622,7 +9616,7 @@
         <v>25</v>
       </c>
       <c r="P36" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -9672,7 +9666,7 @@
         <v>25</v>
       </c>
       <c r="P37" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -9722,7 +9716,7 @@
         <v>25</v>
       </c>
       <c r="P38" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -9772,7 +9766,7 @@
         <v>25</v>
       </c>
       <c r="P39" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -9822,7 +9816,7 @@
         <v>25</v>
       </c>
       <c r="P40" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -9872,7 +9866,7 @@
         <v>25</v>
       </c>
       <c r="P41" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -9922,7 +9916,7 @@
         <v>25</v>
       </c>
       <c r="P42" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -9972,7 +9966,7 @@
         <v>25</v>
       </c>
       <c r="P43" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -10022,7 +10016,7 @@
         <v>25</v>
       </c>
       <c r="P44" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -10072,7 +10066,7 @@
         <v>25</v>
       </c>
       <c r="P45" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -10122,7 +10116,7 @@
         <v>25</v>
       </c>
       <c r="P46" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -10172,7 +10166,7 @@
         <v>25</v>
       </c>
       <c r="P47" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -10222,7 +10216,7 @@
         <v>25</v>
       </c>
       <c r="P48" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -10272,7 +10266,7 @@
         <v>25</v>
       </c>
       <c r="P49" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -10322,7 +10316,7 @@
         <v>25</v>
       </c>
       <c r="P50" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -10372,7 +10366,7 @@
         <v>25</v>
       </c>
       <c r="P51" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -10422,7 +10416,7 @@
         <v>25</v>
       </c>
       <c r="P52" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -10472,7 +10466,7 @@
         <v>25</v>
       </c>
       <c r="P53" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -10522,7 +10516,7 @@
         <v>25</v>
       </c>
       <c r="P54" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -10572,7 +10566,7 @@
         <v>25</v>
       </c>
       <c r="P55" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -10622,7 +10616,7 @@
         <v>25</v>
       </c>
       <c r="P56" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -10672,7 +10666,7 @@
         <v>25</v>
       </c>
       <c r="P57" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -10722,7 +10716,7 @@
         <v>25</v>
       </c>
       <c r="P58" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -10772,7 +10766,7 @@
         <v>25</v>
       </c>
       <c r="P59" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -10822,7 +10816,7 @@
         <v>25</v>
       </c>
       <c r="P60" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -10872,7 +10866,7 @@
         <v>25</v>
       </c>
       <c r="P61" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -10922,7 +10916,7 @@
         <v>25</v>
       </c>
       <c r="P62" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -10972,7 +10966,7 @@
         <v>25</v>
       </c>
       <c r="P63" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -11022,7 +11016,7 @@
         <v>25</v>
       </c>
       <c r="P64" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -11072,7 +11066,7 @@
         <v>25</v>
       </c>
       <c r="P65" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -11122,7 +11116,7 @@
         <v>25</v>
       </c>
       <c r="P66" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -11172,7 +11166,7 @@
         <v>25</v>
       </c>
       <c r="P67" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -11222,7 +11216,7 @@
         <v>25</v>
       </c>
       <c r="P68" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:16">
@@ -11272,7 +11266,7 @@
         <v>25</v>
       </c>
       <c r="P69" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -11322,7 +11316,7 @@
         <v>25</v>
       </c>
       <c r="P70" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:16">
@@ -11372,7 +11366,7 @@
         <v>25</v>
       </c>
       <c r="P71" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -11422,7 +11416,7 @@
         <v>25</v>
       </c>
       <c r="P72" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:16">
@@ -11472,7 +11466,7 @@
         <v>25</v>
       </c>
       <c r="P73" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -11522,7 +11516,7 @@
         <v>25</v>
       </c>
       <c r="P74" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -11572,7 +11566,7 @@
         <v>25</v>
       </c>
       <c r="P75" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -11622,7 +11616,7 @@
         <v>25</v>
       </c>
       <c r="P76" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -11672,7 +11666,7 @@
         <v>25</v>
       </c>
       <c r="P77" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -11722,7 +11716,7 @@
         <v>25</v>
       </c>
       <c r="P78" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -11772,7 +11766,7 @@
         <v>25</v>
       </c>
       <c r="P79" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -11822,7 +11816,7 @@
         <v>25</v>
       </c>
       <c r="P80" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -11872,7 +11866,7 @@
         <v>25</v>
       </c>
       <c r="P81" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -11922,7 +11916,7 @@
         <v>25</v>
       </c>
       <c r="P82" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -11972,7 +11966,7 @@
         <v>25</v>
       </c>
       <c r="P83" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -12022,7 +12016,7 @@
         <v>25</v>
       </c>
       <c r="P84" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -12072,7 +12066,7 @@
         <v>25</v>
       </c>
       <c r="P85" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -12122,7 +12116,7 @@
         <v>25</v>
       </c>
       <c r="P86" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -12172,7 +12166,7 @@
         <v>25</v>
       </c>
       <c r="P87" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -12222,7 +12216,7 @@
         <v>25</v>
       </c>
       <c r="P88" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -12272,7 +12266,7 @@
         <v>25</v>
       </c>
       <c r="P89" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -12322,7 +12316,7 @@
         <v>25</v>
       </c>
       <c r="P90" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -12372,7 +12366,7 @@
         <v>25</v>
       </c>
       <c r="P91" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -12422,7 +12416,7 @@
         <v>25</v>
       </c>
       <c r="P92" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -12472,7 +12466,7 @@
         <v>25</v>
       </c>
       <c r="P93" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -12522,7 +12516,7 @@
         <v>25</v>
       </c>
       <c r="P94" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -12572,7 +12566,7 @@
         <v>25</v>
       </c>
       <c r="P95" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:16">
@@ -12622,7 +12616,7 @@
         <v>25</v>
       </c>
       <c r="P96" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:16">
@@ -12672,7 +12666,7 @@
         <v>25</v>
       </c>
       <c r="P97" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:16">
@@ -12722,7 +12716,7 @@
         <v>25</v>
       </c>
       <c r="P98" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="99" spans="1:16">
@@ -12772,7 +12766,7 @@
         <v>25</v>
       </c>
       <c r="P99" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:16">
@@ -12822,7 +12816,7 @@
         <v>25</v>
       </c>
       <c r="P100" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -12872,7 +12866,7 @@
         <v>25</v>
       </c>
       <c r="P101" t="s">
-        <v>339</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -12988,8 +12982,8 @@
   <sheetPr/>
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -13094,7 +13088,7 @@
         <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -13144,7 +13138,7 @@
         <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -13194,7 +13188,7 @@
         <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -13244,7 +13238,7 @@
         <v>25</v>
       </c>
       <c r="P5" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -13294,7 +13288,7 @@
         <v>25</v>
       </c>
       <c r="P6" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -13344,7 +13338,7 @@
         <v>25</v>
       </c>
       <c r="P7" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -13394,7 +13388,7 @@
         <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -13444,7 +13438,7 @@
         <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -13494,7 +13488,7 @@
         <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -13544,7 +13538,7 @@
         <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -13594,7 +13588,7 @@
         <v>25</v>
       </c>
       <c r="P12" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -13644,7 +13638,7 @@
         <v>25</v>
       </c>
       <c r="P13" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -13694,7 +13688,7 @@
         <v>25</v>
       </c>
       <c r="P14" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -13744,7 +13738,7 @@
         <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -13794,7 +13788,7 @@
         <v>25</v>
       </c>
       <c r="P16" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -13844,7 +13838,7 @@
         <v>25</v>
       </c>
       <c r="P17" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -13894,7 +13888,7 @@
         <v>25</v>
       </c>
       <c r="P18" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -13944,7 +13938,7 @@
         <v>25</v>
       </c>
       <c r="P19" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -13994,7 +13988,7 @@
         <v>25</v>
       </c>
       <c r="P20" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -14044,7 +14038,7 @@
         <v>25</v>
       </c>
       <c r="P21" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -14094,7 +14088,7 @@
         <v>25</v>
       </c>
       <c r="P22" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -14144,7 +14138,7 @@
         <v>25</v>
       </c>
       <c r="P23" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -14194,7 +14188,7 @@
         <v>25</v>
       </c>
       <c r="P24" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -14244,7 +14238,7 @@
         <v>25</v>
       </c>
       <c r="P25" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -14294,7 +14288,7 @@
         <v>25</v>
       </c>
       <c r="P26" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -14344,7 +14338,7 @@
         <v>25</v>
       </c>
       <c r="P27" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -14394,7 +14388,7 @@
         <v>25</v>
       </c>
       <c r="P28" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -14444,7 +14438,7 @@
         <v>25</v>
       </c>
       <c r="P29" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -14494,7 +14488,7 @@
         <v>25</v>
       </c>
       <c r="P30" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -14544,7 +14538,7 @@
         <v>25</v>
       </c>
       <c r="P31" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -14594,7 +14588,7 @@
         <v>25</v>
       </c>
       <c r="P32" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -14644,7 +14638,7 @@
         <v>25</v>
       </c>
       <c r="P33" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -14694,7 +14688,7 @@
         <v>25</v>
       </c>
       <c r="P34" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -14744,7 +14738,7 @@
         <v>25</v>
       </c>
       <c r="P35" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -14794,7 +14788,7 @@
         <v>25</v>
       </c>
       <c r="P36" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -14844,7 +14838,7 @@
         <v>25</v>
       </c>
       <c r="P37" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -14894,7 +14888,7 @@
         <v>25</v>
       </c>
       <c r="P38" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -14944,7 +14938,7 @@
         <v>25</v>
       </c>
       <c r="P39" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -14994,7 +14988,7 @@
         <v>25</v>
       </c>
       <c r="P40" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -15044,7 +15038,7 @@
         <v>25</v>
       </c>
       <c r="P41" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -15094,7 +15088,7 @@
         <v>25</v>
       </c>
       <c r="P42" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -15144,7 +15138,7 @@
         <v>25</v>
       </c>
       <c r="P43" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -15194,7 +15188,7 @@
         <v>25</v>
       </c>
       <c r="P44" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -15244,7 +15238,7 @@
         <v>25</v>
       </c>
       <c r="P45" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -15294,7 +15288,7 @@
         <v>25</v>
       </c>
       <c r="P46" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -15344,7 +15338,7 @@
         <v>25</v>
       </c>
       <c r="P47" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -15394,7 +15388,7 @@
         <v>25</v>
       </c>
       <c r="P48" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -15444,7 +15438,7 @@
         <v>25</v>
       </c>
       <c r="P49" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -15494,7 +15488,7 @@
         <v>25</v>
       </c>
       <c r="P50" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -15544,7 +15538,7 @@
         <v>25</v>
       </c>
       <c r="P51" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -15594,7 +15588,7 @@
         <v>25</v>
       </c>
       <c r="P52" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -15644,7 +15638,7 @@
         <v>25</v>
       </c>
       <c r="P53" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -15694,7 +15688,7 @@
         <v>25</v>
       </c>
       <c r="P54" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -15744,7 +15738,7 @@
         <v>25</v>
       </c>
       <c r="P55" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -15794,7 +15788,7 @@
         <v>25</v>
       </c>
       <c r="P56" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -15844,7 +15838,7 @@
         <v>25</v>
       </c>
       <c r="P57" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -15894,7 +15888,7 @@
         <v>25</v>
       </c>
       <c r="P58" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -15944,7 +15938,7 @@
         <v>25</v>
       </c>
       <c r="P59" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -15994,7 +15988,7 @@
         <v>25</v>
       </c>
       <c r="P60" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -16044,7 +16038,7 @@
         <v>25</v>
       </c>
       <c r="P61" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -16094,7 +16088,7 @@
         <v>25</v>
       </c>
       <c r="P62" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -16144,7 +16138,7 @@
         <v>25</v>
       </c>
       <c r="P63" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -16194,7 +16188,7 @@
         <v>25</v>
       </c>
       <c r="P64" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -16244,7 +16238,7 @@
         <v>25</v>
       </c>
       <c r="P65" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -16294,7 +16288,7 @@
         <v>25</v>
       </c>
       <c r="P66" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -16344,7 +16338,7 @@
         <v>25</v>
       </c>
       <c r="P67" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -16394,7 +16388,7 @@
         <v>25</v>
       </c>
       <c r="P68" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:16">
@@ -16444,7 +16438,7 @@
         <v>25</v>
       </c>
       <c r="P69" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -16494,7 +16488,7 @@
         <v>25</v>
       </c>
       <c r="P70" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:16">
@@ -16544,7 +16538,7 @@
         <v>25</v>
       </c>
       <c r="P71" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -16594,7 +16588,7 @@
         <v>25</v>
       </c>
       <c r="P72" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:16">
@@ -16644,7 +16638,7 @@
         <v>25</v>
       </c>
       <c r="P73" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -16694,7 +16688,7 @@
         <v>25</v>
       </c>
       <c r="P74" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -16744,7 +16738,7 @@
         <v>25</v>
       </c>
       <c r="P75" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -16794,7 +16788,7 @@
         <v>25</v>
       </c>
       <c r="P76" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -16844,7 +16838,7 @@
         <v>25</v>
       </c>
       <c r="P77" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -16894,7 +16888,7 @@
         <v>25</v>
       </c>
       <c r="P78" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -16944,7 +16938,7 @@
         <v>25</v>
       </c>
       <c r="P79" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -16994,7 +16988,7 @@
         <v>25</v>
       </c>
       <c r="P80" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -17044,7 +17038,7 @@
         <v>25</v>
       </c>
       <c r="P81" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -17094,7 +17088,7 @@
         <v>25</v>
       </c>
       <c r="P82" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -17144,7 +17138,7 @@
         <v>25</v>
       </c>
       <c r="P83" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -17194,7 +17188,7 @@
         <v>25</v>
       </c>
       <c r="P84" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -17244,7 +17238,7 @@
         <v>25</v>
       </c>
       <c r="P85" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -17294,7 +17288,7 @@
         <v>25</v>
       </c>
       <c r="P86" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -17344,7 +17338,7 @@
         <v>25</v>
       </c>
       <c r="P87" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -17394,7 +17388,7 @@
         <v>25</v>
       </c>
       <c r="P88" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -17444,7 +17438,7 @@
         <v>25</v>
       </c>
       <c r="P89" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -17494,7 +17488,7 @@
         <v>25</v>
       </c>
       <c r="P90" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -17544,7 +17538,7 @@
         <v>25</v>
       </c>
       <c r="P91" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -17594,7 +17588,7 @@
         <v>25</v>
       </c>
       <c r="P92" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -17644,7 +17638,7 @@
         <v>25</v>
       </c>
       <c r="P93" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -17694,7 +17688,7 @@
         <v>25</v>
       </c>
       <c r="P94" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -17744,7 +17738,7 @@
         <v>25</v>
       </c>
       <c r="P95" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:16">
@@ -17794,7 +17788,7 @@
         <v>25</v>
       </c>
       <c r="P96" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:16">
@@ -17844,7 +17838,7 @@
         <v>25</v>
       </c>
       <c r="P97" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:16">
@@ -17894,7 +17888,7 @@
         <v>25</v>
       </c>
       <c r="P98" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:16">
@@ -17944,7 +17938,7 @@
         <v>25</v>
       </c>
       <c r="P99" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:16">
@@ -17994,7 +17988,7 @@
         <v>25</v>
       </c>
       <c r="P100" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -18044,7 +18038,7 @@
         <v>25</v>
       </c>
       <c r="P101" t="s">
-        <v>339</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -28504,14 +28498,15 @@
   <sheetPr/>
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="17.287037037037" customWidth="1"/>
     <col min="14" max="14" width="16.5740740740741" customWidth="1"/>
+    <col min="16" max="16" width="11.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -33677,8 +33672,8 @@
   <sheetPr/>
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -38850,13 +38845,14 @@
   <sheetPr/>
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="14" max="14" width="11.7777777777778" customWidth="1"/>
     <col min="16" max="16" width="16.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
@@ -44023,8 +44019,8 @@
   <sheetPr/>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -49500,13 +49496,14 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="17.287037037037" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -54976,7 +54973,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -75987,13 +75984,14 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="P2" sqref="P2:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="17.287037037037" customWidth="1"/>
     <col min="15" max="15" width="14.5740740740741" customWidth="1"/>
+    <col min="16" max="16" width="11.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>